<commit_message>
Save the esconnector.HoldingData in es instead of stock.Holding
</commit_message>
<xml_diff>
--- a/resource/ARK.xlsx
+++ b/resource/ARK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15902\go\src\github.com\skeyic\ark-robot\data\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15902\go\src\github.com\skeyic\ark-robot\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB83C29C-20C6-4C75-8EE7-1C9815244A9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FA7A20-25AA-46D5-BF6A-28819F8A1A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F07BBE50-B47C-4F49-968F-328D3756EA4F}"/>
+    <workbookView xWindow="9720" yWindow="165" windowWidth="28035" windowHeight="20475" xr2:uid="{F07BBE50-B47C-4F49-968F-328D3756EA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -33,17 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Shards</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ARKK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSLA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -163,14 +155,6 @@
   </si>
   <si>
     <t>EXAMPLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>88160R101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>”TESLA INC“</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -570,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EB39C5-F66E-4865-A96F-E3BCE74C61CA}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -596,33 +580,33 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N1" s="7"/>
     </row>
@@ -632,16 +616,16 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="3">
@@ -654,30 +638,30 @@
         <v>44250</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="99" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1">
         <v>1000</v>
@@ -686,36 +670,22 @@
         <v>0.1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N3" s="6">
         <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>